<commit_message>
PROS-6182 - MARSRU - KPI logic change
</commit_message>
<xml_diff>
--- a/Projects/MARSRU_PROD/Data/MARS KPIs.xlsx
+++ b/Projects/MARSRU_PROD/Data/MARS KPIs.xlsx
@@ -13,7 +13,7 @@
     <sheet name="2306 Automatic - Backup-2018-06" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPI!$B$1:$AA$72</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
@@ -28,6 +28,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">KPI!$B$1:$AA$71</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -634,23 +635,23 @@
   </si>
   <si>
     <t xml:space="preserve">form_factor: POUCH, pouch, Pouch. brand_name: Kitekat
-brand_name: Friskies
+form_factor: POUCH, pouch, Pouch. brand_name: Friskies
 1.5
 OR
 form_factor: POUCH, pouch, Pouch. brand_name: Kitekat
-brand_name: TomCat
+form_factor: POUCH, pouch, Pouch. brand_name: TomCat
 1.5
 OR
 form_factor: POUCH, pouch, Pouch. brand_name: Kitekat
-brand_name: Lenta
+form_factor: POUCH, pouch, Pouch. brand_name: Lenta
 1.5
 OR
 form_factor: POUCH, pouch, Pouch. brand_name: Kitekat
-brand_name: Catty
+form_factor: POUCH, pouch, Pouch. brand_name: Catty
 1.5
 OR
 form_factor: POUCH, pouch, Pouch. brand_name: Kitekat
-brand_name: Dars
+form_factor: POUCH, pouch, Pouch. brand_name: Dars
 1.5</t>
   </si>
   <si>
@@ -661,7 +662,7 @@
   </si>
   <si>
     <t xml:space="preserve">form_factor: POUCH, pouch, Pouch. brand_name: Whiskas. exclude sub_category: C&amp;T. exclude product_fk: 673,674,675,676
-brand_name: Felix
+form_factor: POUCH, pouch, Pouch. brand_name: Felix
 1.3</t>
   </si>
   <si>
@@ -672,8 +673,8 @@
     <t xml:space="preserve">To return true if total linear length of WET POUCHES PF+SHEBA &gt;= 130%*any of list of brands {Gourmet}</t>
   </si>
   <si>
-    <t xml:space="preserve">form_factor: POUCH, pouch, Pouch. brand_name: Perfect Fit, Sheba
-brand_name: Gourmet
+    <t xml:space="preserve">form_factor: POUCH, pouch, Pouch, CANS, can, Can. brand_name: Perfect Fit, Sheba
+form_factor: POUCH, pouch, Pouch, CANS, can, Can. Brand_name: Gourmet
 1.3</t>
   </si>
   <si>
@@ -1224,39 +1225,38 @@
   </sheetPr>
   <dimension ref="A1:AA65536"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="P63" activeCellId="0" sqref="P63"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="78" zoomScaleNormal="78" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="29.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="87.1943319838057"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="89.9797570850202"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.2105263157895"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="33.6356275303644"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="3" width="15.6396761133603"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="33.1012145748988"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="18" min="17" style="2" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="20" min="19" style="2" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="14.7813765182186"/>
-    <col collapsed="false" hidden="false" max="23" min="22" style="2" width="16.0688259109312"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="20.246963562753"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="50.8825910931174"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="15.5303643724696"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="1025" min="28" style="0" width="10.6032388663968"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.9919028340081"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.42914979757085"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.7125506072875"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="91.1214574898785"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="35.7044534412955"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="21.8542510121457"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="21.5668016194332"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="2" width="94.1214574898785"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="15.7125506072875"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="35.1336032388664"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="3" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="3" width="34.5627530364372"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="15.2834008097166"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="2" width="15.2834008097166"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="2" width="19.4251012145749"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="2" width="15.2834008097166"/>
+    <col collapsed="false" hidden="false" max="23" min="22" style="2" width="16.7125506072875"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="2" width="21.1376518218623"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="2" width="53.1295546558704"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="2" width="16.2834008097166"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="2" width="19.8542510121458"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="108.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -5343,7 +5343,7 @@
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <autoFilter ref="B1:AA71"/>
+  <autoFilter ref="B1:AA72"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -5368,10 +5368,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.85425101214575"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1417004048583"/>
+    <col collapsed="false" hidden="false" max="5" min="3" style="0" width="10.995951417004"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5483,9 +5483,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="16" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="16" min="1" style="0" width="8.85425101214575"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="20.5668016194332"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="8.85425101214575"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="89.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>